<commit_message>
second commit / 20170517
</commit_message>
<xml_diff>
--- a/price_excel/prdt_paper_price_excel.xlsx
+++ b/price_excel/prdt_paper_price_excel.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\★디프린팅3.0\08.계산형(판매)정의서\01.종이\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7710"/>
+    <workbookView xWindow="630" yWindow="600" windowWidth="19095" windowHeight="8550"/>
   </bookViews>
   <sheets>
-    <sheet name="마메이드" sheetId="1" r:id="rId1"/>
+    <sheet name="홍승현에바그린지" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
@@ -30,22 +25,25 @@
     <t>종이분류</t>
   </si>
   <si>
-    <t>특수용지</t>
+    <t>기타용지</t>
   </si>
   <si>
     <t>종이</t>
   </si>
   <si>
-    <t>마메이드!-!백색</t>
+    <t>홍승현에바그린지!네추럴!미색</t>
   </si>
   <si>
     <t>계열</t>
   </si>
   <si>
+    <t>국</t>
+  </si>
+  <si>
     <t>사이즈</t>
   </si>
   <si>
-    <t>1091*788</t>
+    <t>939*636</t>
   </si>
   <si>
     <t>기준단위</t>
@@ -69,10 +67,7 @@
     <t>판매가격</t>
   </si>
   <si>
-    <t>244g</t>
-  </si>
-  <si>
-    <t>407g</t>
+    <t>190g</t>
   </si>
 </sst>
 </file>
@@ -130,7 +125,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -268,41 +263,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thick">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="dotted">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="dotted">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="dotted">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="dotted">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thick">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="dotted">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="dotted">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -330,18 +295,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -362,9 +315,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -657,10 +607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -673,91 +623,91 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="17"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="13"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="17"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="13"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="17"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="13"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="15">
-        <v>46</v>
-      </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="17"/>
+      <c r="B4" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="13"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="17"/>
+      <c r="B5" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="13"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="17"/>
+      <c r="B6" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="13"/>
     </row>
     <row r="7" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B8" s="7">
-        <v>1015000</v>
+        <v>180000</v>
       </c>
       <c r="C8" s="9">
         <v>0</v>
@@ -767,25 +717,7 @@
       </c>
       <c r="E8" s="10">
         <f>((C8/100)*B8)+B8+D8</f>
-        <v>1015000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="11">
-        <v>1693000</v>
-      </c>
-      <c r="C9" s="13">
-        <v>0</v>
-      </c>
-      <c r="D9" s="12">
-        <v>0</v>
-      </c>
-      <c r="E9" s="14">
-        <f>((C9/100)*B9)+B9+D9</f>
-        <v>1693000</v>
+        <v>180000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>